<commit_message>
- added some extra data to the example of filled template
</commit_message>
<xml_diff>
--- a/template_v4_DatasetExample.xlsx
+++ b/template_v4_DatasetExample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adam/PycharmProjects/ULTERA-contribute/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F90961D3-1803-E04D-B450-3E0BF26FADD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD1939D1-6A67-7B41-BA20-173BA948657A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="151">
   <si>
     <t>Name:</t>
   </si>
@@ -436,6 +436,138 @@
   </si>
   <si>
     <t>T7 / F6 / P13</t>
+  </si>
+  <si>
+    <t>CoCrFeNi</t>
+  </si>
+  <si>
+    <t>all YS recorded as +1 MPa grain size:150-200micrometers</t>
+  </si>
+  <si>
+    <t>tensile ductility</t>
+  </si>
+  <si>
+    <t>10.1016/j.intermet.2015.01.004</t>
+  </si>
+  <si>
+    <t>CoCrFeNiMo0.2</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>10.3390/e21050448</t>
+  </si>
+  <si>
+    <t>CoNiFe</t>
+  </si>
+  <si>
+    <t>CW+A</t>
+  </si>
+  <si>
+    <t>fixed elongation grain size:74micrometers</t>
+  </si>
+  <si>
+    <t>10.1016/j.intermet.2019.106477</t>
+  </si>
+  <si>
+    <t>FeCrCoMnNi</t>
+  </si>
+  <si>
+    <t>CW + A</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> grain size:8micrometers</t>
+  </si>
+  <si>
+    <t>10.1016/j.msea.2019.04.025</t>
+  </si>
+  <si>
+    <t>Co20.6Cr19.9Fe19.5Ni20.9Mn19.1</t>
+  </si>
+  <si>
+    <t>fixed grain size; wrong unit grain size:17.1micrometers</t>
+  </si>
+  <si>
+    <t>10.1016/j.msea.2019.01.112</t>
+  </si>
+  <si>
+    <t>FeCoNiCrTi0.2</t>
+  </si>
+  <si>
+    <t>missed the ductility values, incorrect processing (from AC to CW + A), grain size to 51</t>
+  </si>
+  <si>
+    <t>10.1016/j.actamat.2018.11.049</t>
+  </si>
+  <si>
+    <t>Lin_2023_SomeNicePaper</t>
+  </si>
+  <si>
+    <t>MPEA-1</t>
+  </si>
+  <si>
+    <t>MPEA-2</t>
+  </si>
+  <si>
+    <t>MPEA-3</t>
+  </si>
+  <si>
+    <t>MPEA-4</t>
+  </si>
+  <si>
+    <t>MPEA-5</t>
+  </si>
+  <si>
+    <t>MPEA-6</t>
+  </si>
+  <si>
+    <t>Ti30 Zr30 Hf16 Nb24</t>
+  </si>
+  <si>
+    <t>tensile yield strength</t>
+  </si>
+  <si>
+    <t>F6</t>
+  </si>
+  <si>
+    <t>10.1016/j.actamat.2023.118728</t>
+  </si>
+  <si>
+    <t>BCC+BCC</t>
+  </si>
+  <si>
+    <t>AC+CR+A</t>
+  </si>
+  <si>
+    <t>20min at 900*C, nanoprecipitate strenghtening (see paper)</t>
+  </si>
+  <si>
+    <t>AC+CR+A+A</t>
+  </si>
+  <si>
+    <t>20min at 900*C + 200h at 600*C</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>SomeID-1</t>
+  </si>
+  <si>
+    <t>SomeID-2</t>
+  </si>
+  <si>
+    <t>SomeID-3</t>
+  </si>
+  <si>
+    <t>SomeID-4</t>
+  </si>
+  <si>
+    <t>SomeID-5</t>
+  </si>
+  <si>
+    <t>SomeID-6</t>
   </si>
 </sst>
 </file>
@@ -1012,7 +1144,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1124,6 +1256,33 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1175,33 +1334,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1486,7 +1619,7 @@
   <dimension ref="A1:T430"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1521,19 +1654,19 @@
       <c r="B2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="46"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="42"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
+      <c r="N2" s="51"/>
       <c r="O2" s="27"/>
     </row>
     <row r="3" spans="1:20" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1543,17 +1676,17 @@
       <c r="B3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="47"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="44"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="52"/>
+      <c r="N3" s="53"/>
       <c r="O3" s="27"/>
     </row>
     <row r="4" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1571,43 +1704,43 @@
       <c r="B5" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="57" t="s">
+      <c r="C5" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="58" t="s">
+      <c r="D5" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="58" t="s">
+      <c r="E5" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="58" t="s">
+      <c r="F5" s="47" t="s">
         <v>102</v>
       </c>
-      <c r="G5" s="58" t="s">
+      <c r="G5" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="65" t="s">
+      <c r="H5" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="I5" s="58" t="s">
+      <c r="I5" s="47" t="s">
         <v>103</v>
       </c>
-      <c r="J5" s="58" t="s">
+      <c r="J5" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="K5" s="58" t="s">
+      <c r="K5" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="L5" s="58" t="s">
+      <c r="L5" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="M5" s="58" t="s">
+      <c r="M5" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="N5" s="58" t="s">
+      <c r="N5" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="O5" s="59" t="s">
+      <c r="O5" s="41" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1618,19 +1751,19 @@
       <c r="B6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="58"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="58"/>
-      <c r="G6" s="58"/>
-      <c r="H6" s="66"/>
-      <c r="I6" s="58"/>
-      <c r="J6" s="58"/>
-      <c r="K6" s="58"/>
-      <c r="L6" s="58"/>
-      <c r="M6" s="58"/>
-      <c r="N6" s="58"/>
-      <c r="O6" s="60"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="47"/>
+      <c r="N6" s="47"/>
+      <c r="O6" s="42"/>
     </row>
     <row r="7" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -1675,7 +1808,7 @@
       <c r="N7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="O7" s="61"/>
+      <c r="O7" s="43"/>
       <c r="P7" s="33" t="s">
         <v>43</v>
       </c>
@@ -1688,35 +1821,35 @@
     </row>
     <row r="8" spans="1:20" ht="20.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="50"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="52" t="s">
+      <c r="C8" s="59"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="53"/>
-      <c r="H8" s="53"/>
-      <c r="I8" s="53"/>
-      <c r="J8" s="54"/>
-      <c r="K8" s="54"/>
-      <c r="L8" s="54"/>
-      <c r="M8" s="55" t="s">
+      <c r="G8" s="62"/>
+      <c r="H8" s="62"/>
+      <c r="I8" s="62"/>
+      <c r="J8" s="63"/>
+      <c r="K8" s="63"/>
+      <c r="L8" s="63"/>
+      <c r="M8" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="N8" s="56"/>
+      <c r="N8" s="65"/>
       <c r="O8" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="P8" s="62" t="s">
+      <c r="P8" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="Q8" s="63"/>
-      <c r="R8" s="63"/>
-      <c r="S8" s="63"/>
-      <c r="T8" s="64"/>
+      <c r="Q8" s="45"/>
+      <c r="R8" s="45"/>
+      <c r="S8" s="45"/>
+      <c r="T8" s="46"/>
     </row>
     <row r="9" spans="1:20" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -2135,7 +2268,9 @@
       <c r="K18" s="34"/>
       <c r="L18" s="40"/>
       <c r="M18" s="40"/>
-      <c r="N18" s="21"/>
+      <c r="N18" s="21" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="21" t="s">
@@ -2159,199 +2294,459 @@
       <c r="K19" s="34"/>
       <c r="L19" s="40"/>
       <c r="M19" s="40"/>
-      <c r="N19" s="21"/>
+      <c r="N19" s="21" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="38"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="35"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="35"/>
+      <c r="A20" s="38" t="s">
+        <v>129</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="C20" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="F20" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="G20" s="35" t="s">
+        <v>21</v>
+      </c>
       <c r="H20" s="35"/>
-      <c r="I20" s="37"/>
-      <c r="J20" s="34"/>
+      <c r="I20" s="37">
+        <v>298</v>
+      </c>
+      <c r="J20" s="34">
+        <v>48</v>
+      </c>
       <c r="K20" s="34"/>
       <c r="L20" s="40"/>
       <c r="M20" s="40"/>
-      <c r="N20" s="21"/>
+      <c r="N20" s="21" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" s="38"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="35"/>
-      <c r="D21" s="35"/>
+      <c r="A21" s="38" t="s">
+        <v>130</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="C21" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" s="35" t="s">
+        <v>112</v>
+      </c>
       <c r="E21" s="21"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="35"/>
+      <c r="F21" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="G21" s="35" t="s">
+        <v>21</v>
+      </c>
       <c r="H21" s="35"/>
-      <c r="I21" s="37"/>
-      <c r="J21" s="34"/>
+      <c r="I21" s="37">
+        <v>298</v>
+      </c>
+      <c r="J21" s="34">
+        <v>47</v>
+      </c>
       <c r="K21" s="34"/>
       <c r="L21" s="40"/>
       <c r="M21" s="21"/>
-      <c r="N21" s="21"/>
+      <c r="N21" s="21" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="38"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="35"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="35"/>
+      <c r="A22" s="38" t="s">
+        <v>131</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="C22" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22" s="35" t="s">
+        <v>115</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="F22" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="G22" s="35" t="s">
+        <v>21</v>
+      </c>
       <c r="H22" s="35"/>
-      <c r="I22" s="37"/>
-      <c r="J22" s="34"/>
+      <c r="I22" s="37">
+        <v>298</v>
+      </c>
+      <c r="J22" s="34">
+        <v>47</v>
+      </c>
       <c r="K22" s="34"/>
       <c r="L22" s="40"/>
       <c r="M22" s="21"/>
-      <c r="N22" s="21"/>
+      <c r="N22" s="21" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" s="38"/>
-      <c r="B23" s="21"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="35"/>
+      <c r="A23" s="38" t="s">
+        <v>132</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="C23" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="D23" s="35" t="s">
+        <v>119</v>
+      </c>
+      <c r="E23" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="F23" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="G23" s="35" t="s">
+        <v>21</v>
+      </c>
       <c r="H23" s="35"/>
-      <c r="I23" s="37"/>
-      <c r="J23" s="34"/>
+      <c r="I23" s="37">
+        <v>298</v>
+      </c>
+      <c r="J23" s="34">
+        <v>47</v>
+      </c>
       <c r="K23" s="34"/>
       <c r="L23" s="40"/>
       <c r="M23" s="21"/>
-      <c r="N23" s="21"/>
+      <c r="N23" s="21" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A24" s="38"/>
-      <c r="B24" s="21"/>
-      <c r="C24" s="35"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="35"/>
+      <c r="A24" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="C24" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" s="35" t="s">
+        <v>115</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="F24" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="G24" s="35" t="s">
+        <v>21</v>
+      </c>
       <c r="H24" s="35"/>
-      <c r="I24" s="37"/>
-      <c r="J24" s="34"/>
+      <c r="I24" s="37">
+        <v>298</v>
+      </c>
+      <c r="J24" s="34">
+        <v>60.5</v>
+      </c>
       <c r="K24" s="34"/>
       <c r="L24" s="40"/>
       <c r="M24" s="21"/>
-      <c r="N24" s="21"/>
+      <c r="N24" s="21" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A25" s="38"/>
-      <c r="B25" s="21"/>
-      <c r="C25" s="35"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="35"/>
+      <c r="A25" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="B25" s="21" t="s">
+        <v>125</v>
+      </c>
+      <c r="C25" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" s="35" t="s">
+        <v>119</v>
+      </c>
+      <c r="E25" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="F25" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="G25" s="35" t="s">
+        <v>21</v>
+      </c>
       <c r="H25" s="35"/>
-      <c r="I25" s="37"/>
-      <c r="J25" s="34"/>
+      <c r="I25" s="37">
+        <v>77</v>
+      </c>
+      <c r="J25" s="34">
+        <v>46</v>
+      </c>
       <c r="K25" s="34"/>
       <c r="L25" s="40"/>
       <c r="M25" s="21"/>
-      <c r="N25" s="21"/>
+      <c r="N25" s="21" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A26" s="38"/>
-      <c r="B26" s="21"/>
-      <c r="C26" s="35"/>
-      <c r="D26" s="35"/>
+      <c r="A26" s="38" t="s">
+        <v>145</v>
+      </c>
+      <c r="B26" t="s">
+        <v>135</v>
+      </c>
+      <c r="C26" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" s="35" t="s">
+        <v>73</v>
+      </c>
       <c r="E26" s="21"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="35"/>
+      <c r="F26" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="G26" s="35" t="s">
+        <v>21</v>
+      </c>
       <c r="H26" s="35"/>
-      <c r="I26" s="37"/>
-      <c r="J26" s="34"/>
+      <c r="I26" s="37">
+        <v>298</v>
+      </c>
+      <c r="J26" s="34">
+        <v>720000000</v>
+      </c>
       <c r="K26" s="34"/>
-      <c r="L26" s="40"/>
-      <c r="M26" s="21"/>
-      <c r="N26" s="21"/>
+      <c r="L26" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="M26" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="N26" s="67" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A27" s="38"/>
-      <c r="B27" s="21"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="35"/>
+      <c r="A27" s="38" t="s">
+        <v>146</v>
+      </c>
+      <c r="B27" t="s">
+        <v>135</v>
+      </c>
+      <c r="C27" s="35" t="s">
+        <v>139</v>
+      </c>
+      <c r="D27" s="35" t="s">
+        <v>140</v>
+      </c>
+      <c r="E27" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="F27" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="G27" s="35" t="s">
+        <v>21</v>
+      </c>
       <c r="H27" s="35"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="34"/>
+      <c r="I27" s="37">
+        <v>298</v>
+      </c>
+      <c r="J27" s="34">
+        <v>800000000</v>
+      </c>
       <c r="K27" s="34"/>
-      <c r="L27" s="40"/>
-      <c r="M27" s="21"/>
-      <c r="N27" s="21"/>
+      <c r="L27" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="M27" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="N27" s="67" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A28" s="38"/>
-      <c r="B28" s="21"/>
-      <c r="C28" s="35"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="35"/>
+      <c r="A28" s="38" t="s">
+        <v>147</v>
+      </c>
+      <c r="B28" t="s">
+        <v>135</v>
+      </c>
+      <c r="C28" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="D28" s="35" t="s">
+        <v>142</v>
+      </c>
+      <c r="E28" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="F28" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="G28" s="35" t="s">
+        <v>21</v>
+      </c>
       <c r="H28" s="35"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="34"/>
+      <c r="I28" s="37">
+        <v>298</v>
+      </c>
+      <c r="J28" s="34">
+        <v>730000000</v>
+      </c>
       <c r="K28" s="34"/>
-      <c r="L28" s="40"/>
-      <c r="M28" s="21"/>
-      <c r="N28" s="21"/>
+      <c r="L28" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="M28" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="N28" s="67" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A29" s="38"/>
-      <c r="B29" s="21"/>
-      <c r="C29" s="35"/>
-      <c r="D29" s="35"/>
+      <c r="A29" s="38" t="s">
+        <v>148</v>
+      </c>
+      <c r="B29" t="s">
+        <v>135</v>
+      </c>
+      <c r="C29" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29" s="35" t="s">
+        <v>73</v>
+      </c>
       <c r="E29" s="21"/>
-      <c r="F29" s="35"/>
-      <c r="G29" s="35"/>
+      <c r="F29" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="G29" s="35" t="s">
+        <v>21</v>
+      </c>
       <c r="H29" s="35"/>
-      <c r="I29" s="37"/>
-      <c r="J29" s="34"/>
+      <c r="I29" s="37">
+        <v>298</v>
+      </c>
+      <c r="J29" s="34">
+        <v>22.4</v>
+      </c>
       <c r="K29" s="34"/>
-      <c r="L29" s="40"/>
-      <c r="M29" s="21"/>
-      <c r="N29" s="21"/>
+      <c r="L29" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="M29" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="N29" s="67" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A30" s="38"/>
-      <c r="B30" s="21"/>
-      <c r="C30" s="35"/>
-      <c r="D30" s="35"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="35"/>
-      <c r="G30" s="35"/>
+      <c r="A30" s="38" t="s">
+        <v>149</v>
+      </c>
+      <c r="B30" t="s">
+        <v>135</v>
+      </c>
+      <c r="C30" s="35" t="s">
+        <v>139</v>
+      </c>
+      <c r="D30" s="35" t="s">
+        <v>140</v>
+      </c>
+      <c r="E30" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="F30" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="G30" s="35" t="s">
+        <v>21</v>
+      </c>
       <c r="H30" s="35"/>
-      <c r="I30" s="37"/>
-      <c r="J30" s="34"/>
+      <c r="I30" s="37">
+        <v>298</v>
+      </c>
+      <c r="J30" s="34">
+        <v>34</v>
+      </c>
       <c r="K30" s="34"/>
-      <c r="L30" s="21"/>
-      <c r="M30" s="21"/>
-      <c r="N30" s="21"/>
+      <c r="L30" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="M30" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="N30" s="67" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A31" s="38"/>
-      <c r="B31" s="21"/>
-      <c r="C31" s="35"/>
-      <c r="D31" s="35"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="35"/>
-      <c r="G31" s="35"/>
+      <c r="A31" s="38" t="s">
+        <v>150</v>
+      </c>
+      <c r="B31" t="s">
+        <v>135</v>
+      </c>
+      <c r="C31" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="D31" s="35" t="s">
+        <v>142</v>
+      </c>
+      <c r="E31" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="F31" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="G31" s="35" t="s">
+        <v>21</v>
+      </c>
       <c r="H31" s="35"/>
-      <c r="I31" s="37"/>
-      <c r="J31" s="34"/>
+      <c r="I31" s="37">
+        <v>298</v>
+      </c>
+      <c r="J31" s="34">
+        <v>25.6</v>
+      </c>
       <c r="K31" s="34"/>
-      <c r="L31" s="21"/>
-      <c r="M31" s="21"/>
-      <c r="N31" s="21"/>
+      <c r="L31" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="M31" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="N31" s="67" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="38"/>
@@ -8270,11 +8665,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="P8:T8"/>
-    <mergeCell ref="M5:M6"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="H5:H6"/>
     <mergeCell ref="F2:N3"/>
     <mergeCell ref="D2:E3"/>
     <mergeCell ref="B8:E8"/>
@@ -8289,12 +8679,19 @@
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="L5:L6"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="P8:T8"/>
+    <mergeCell ref="M5:M6"/>
+    <mergeCell ref="N5:N6"/>
+    <mergeCell ref="H5:H6"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{D357D88A-2775-40B2-B73F-2173296B7938}"/>
+    <hyperlink ref="N26" r:id="rId2" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.actamat.2023.118728" xr:uid="{745ACDCF-C4C9-FE40-A10E-2C0A27F035B9}"/>
+    <hyperlink ref="N27:N31" r:id="rId3" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.actamat.2023.118728" xr:uid="{5CB04322-CDBF-9940-BC0A-C420A75B37AF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>